<commit_message>
XLSX Get File Comments Adding
</commit_message>
<xml_diff>
--- a/files/simcards.xlsx
+++ b/files/simcards.xlsx
@@ -6,6 +6,116 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
 </workbook>
+</file>
+
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>undefined</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0">
+      <text>
+        <t>شماره سیمکارت</t>
+      </text>
+    </comment>
+    <comment ref="B1" authorId="0">
+      <text>
+        <t>شماره سیمکارت</t>
+      </text>
+    </comment>
+    <comment ref="C1" authorId="0">
+      <text>
+        <t>شماره سیمکارت</t>
+      </text>
+    </comment>
+    <comment ref="D1" authorId="0">
+      <text>
+        <t>شماره سیمکارت</t>
+      </text>
+    </comment>
+    <comment ref="E1" authorId="0">
+      <text>
+        <t>شماره سیمکارت</t>
+      </text>
+    </comment>
+    <comment ref="F1" authorId="0">
+      <text>
+        <t>شماره سیمکارت</t>
+      </text>
+    </comment>
+    <comment ref="G1" authorId="0">
+      <text>
+        <t>شماره سیمکارت</t>
+      </text>
+    </comment>
+    <comment ref="H1" authorId="0">
+      <text>
+        <t>شماره سیمکارت</t>
+      </text>
+    </comment>
+    <comment ref="I1" authorId="0">
+      <text>
+        <t>شماره سیمکارت</t>
+      </text>
+    </comment>
+    <comment ref="J1" authorId="0">
+      <text>
+        <t>شماره سیمکارت</t>
+      </text>
+    </comment>
+    <comment ref="K1" authorId="0">
+      <text>
+        <t>شماره سیمکارت</t>
+      </text>
+    </comment>
+    <comment ref="L1" authorId="0">
+      <text>
+        <t>شماره سیمکارت</t>
+      </text>
+    </comment>
+    <comment ref="M1" authorId="0">
+      <text>
+        <t>شماره سیمکارت</t>
+      </text>
+    </comment>
+    <comment ref="N1" authorId="0">
+      <text>
+        <t>شماره سیمکارت</t>
+      </text>
+    </comment>
+    <comment ref="O1" authorId="0">
+      <text>
+        <t>شماره سیمکارت</t>
+      </text>
+    </comment>
+    <comment ref="P1" authorId="0">
+      <text>
+        <t>شماره سیمکارت</t>
+      </text>
+    </comment>
+    <comment ref="Q1" authorId="0">
+      <text>
+        <t>شماره سیمکارت</t>
+      </text>
+    </comment>
+    <comment ref="R1" authorId="0">
+      <text>
+        <t>شماره سیمکارت</t>
+      </text>
+    </comment>
+    <comment ref="S1" authorId="0">
+      <text>
+        <t>شماره سیمکارت</t>
+      </text>
+    </comment>
+    <comment ref="T1" authorId="0">
+      <text>
+        <t>شماره سیمکارت</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
@@ -64,8 +174,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -465,70 +576,68 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="str">
-        <v>numbers</v>
+      <c r="A2">
+        <v>9374905487</v>
       </c>
       <c r="B2" t="str">
-        <v>khanaei</v>
-      </c>
-      <c r="C2" t="str">
-        <v>price</v>
-      </c>
-      <c r="D2" t="str">
-        <v>maxGhestCount</v>
-      </c>
-      <c r="E2" t="str">
-        <v>pish</v>
-      </c>
-      <c r="F2" t="str">
-        <v>seller</v>
-      </c>
-      <c r="G2" t="str">
-        <v>sellerID</v>
+        <v>0937 490 5487</v>
+      </c>
+      <c r="C2">
+        <v>25000</v>
+      </c>
+      <c r="D2">
+        <v>4</v>
+      </c>
+      <c r="E2">
+        <v>2500</v>
+      </c>
+      <c r="F2">
+        <v>3</v>
       </c>
       <c r="H2" t="str">
-        <v>label</v>
+        <v>فوری</v>
       </c>
       <c r="I2" t="str">
-        <v>description</v>
+        <v>لورم ایپسوم متن ساختگی با تولید سادگی نامفهوم از صنعت چاپ، و با استفاده از طراحان گرافیک است، چاپگرها و متون بلکه روزنامه و مجله در ستون و سطرآنچنان که لازم است، و برای شرایط فعلی تکنولوژی مورد نیاز، و کاربردهای متنوع با هدف بهبود ابزارهای کاربردی می باشد، کتابهای زیادی در شصت و سه درصد گذشته حال و آینده، شناخت فراوان جامعه و متخصصان را می طلبد، تا با نرم افزارها شناخت بیشتری را برای طراحان رایانه ای علی الخصوص طراحان خلاقی، و فرهنگ پیشرو در زبان فارسی ایجاد کرد، در این صورت می توان امید داشت که تمام و دشواری موجود در ارائه راهکارها، و شرایط سخت تایپ به پایان رسد و زمان مورد نیاز شامل حروفچینی دستاوردهای اصلی، و جوابگوی سوالات پیوسته اهل دنیای موجود طراحی اساسا مورد استفاده قرار گیرد.</v>
       </c>
       <c r="J2" t="str">
-        <v>readingType</v>
+        <v>آینه ای</v>
       </c>
       <c r="K2" t="str">
-        <v>operatorName</v>
-      </c>
-      <c r="L2" t="str">
-        <v>activationDate</v>
-      </c>
-      <c r="M2" t="str">
-        <v>isActivated</v>
-      </c>
-      <c r="N2" t="str">
-        <v>ghesti</v>
+        <v>Hamrah-e Aval</v>
+      </c>
+      <c r="L2" s="1">
+        <v>45300.14634259259</v>
+      </c>
+      <c r="M2" t="b">
+        <v>1</v>
+      </c>
+      <c r="N2" t="b">
+        <v>1</v>
       </c>
       <c r="O2" t="str">
-        <v>vaziat</v>
-      </c>
-      <c r="P2" t="str">
-        <v>isVIP</v>
+        <v>used</v>
+      </c>
+      <c r="P2" t="b">
+        <v>1</v>
       </c>
       <c r="Q2" t="str">
-        <v>_id</v>
-      </c>
-      <c r="R2" t="str">
-        <v>createdAt</v>
-      </c>
-      <c r="S2" t="str">
-        <v>updatedAt</v>
-      </c>
-      <c r="T2" t="str">
-        <v>__v</v>
+        <v>6598e4d0c70f02721933a2be</v>
+      </c>
+      <c r="R2" s="1">
+        <v>45297.37393828703</v>
+      </c>
+      <c r="S2" s="1">
+        <v>45297.37916582176</v>
+      </c>
+      <c r="T2">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
     <ignoredError numberStoredAsText="1" sqref="A1:T2"/>
   </ignoredErrors>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
excel export import implemented
</commit_message>
<xml_diff>
--- a/files/simcards.xlsx
+++ b/files/simcards.xlsx
@@ -21,97 +21,97 @@
     </comment>
     <comment ref="B1" authorId="0">
       <text>
-        <t>شماره سیمکارت</t>
+        <t>خانه‌ای</t>
       </text>
     </comment>
     <comment ref="C1" authorId="0">
       <text>
-        <t>شماره سیمکارت</t>
+        <t>قیمت</t>
       </text>
     </comment>
     <comment ref="D1" authorId="0">
       <text>
-        <t>شماره سیمکارت</t>
+        <t>تعداد اقساط حداکثر</t>
       </text>
     </comment>
     <comment ref="E1" authorId="0">
       <text>
-        <t>شماره سیمکارت</t>
+        <t>پیش</t>
       </text>
     </comment>
     <comment ref="F1" authorId="0">
       <text>
-        <t>شماره سیمکارت</t>
+        <t>فروشنده</t>
       </text>
     </comment>
     <comment ref="G1" authorId="0">
       <text>
-        <t>شماره سیمکارت</t>
+        <t>شناسه فروشنده</t>
       </text>
     </comment>
     <comment ref="H1" authorId="0">
       <text>
-        <t>شماره سیمکارت</t>
+        <t>برچسب</t>
       </text>
     </comment>
     <comment ref="I1" authorId="0">
       <text>
-        <t>شماره سیمکارت</t>
+        <t>توضیحات</t>
       </text>
     </comment>
     <comment ref="J1" authorId="0">
       <text>
-        <t>شماره سیمکارت</t>
+        <t>نوع خواندن</t>
       </text>
     </comment>
     <comment ref="K1" authorId="0">
       <text>
-        <t>شماره سیمکارت</t>
+        <t>نام اپراتور</t>
       </text>
     </comment>
     <comment ref="L1" authorId="0">
       <text>
-        <t>شماره سیمکارت</t>
+        <t>تاریخ فعالسازی</t>
       </text>
     </comment>
     <comment ref="M1" authorId="0">
       <text>
-        <t>شماره سیمکارت</t>
+        <t>فعال شده</t>
       </text>
     </comment>
     <comment ref="N1" authorId="0">
       <text>
-        <t>شماره سیمکارت</t>
+        <t>قسطی</t>
       </text>
     </comment>
     <comment ref="O1" authorId="0">
       <text>
-        <t>شماره سیمکارت</t>
+        <t>وضعیت</t>
       </text>
     </comment>
     <comment ref="P1" authorId="0">
       <text>
-        <t>شماره سیمکارت</t>
+        <t>ویژه</t>
       </text>
     </comment>
     <comment ref="Q1" authorId="0">
       <text>
-        <t>شماره سیمکارت</t>
+        <t>شناسه</t>
       </text>
     </comment>
     <comment ref="R1" authorId="0">
       <text>
-        <t>شماره سیمکارت</t>
+        <t>تاریخ ایجاد</t>
       </text>
     </comment>
     <comment ref="S1" authorId="0">
       <text>
-        <t>شماره سیمکارت</t>
+        <t>تاریخ به‌روزرسانی</t>
       </text>
     </comment>
     <comment ref="T1" authorId="0">
       <text>
-        <t>شماره سیمکارت</t>
+        <t>نسخه</t>
       </text>
     </comment>
   </commentList>
@@ -508,7 +508,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:T2"/>
+  <dimension ref="A1:T20"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -577,66 +577,1071 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>9374905487</v>
+        <v>9125004900</v>
       </c>
       <c r="B2" t="str">
-        <v>0937 490 5487</v>
+        <v>0912  500 4900</v>
       </c>
       <c r="C2">
-        <v>25000</v>
+        <v>7500</v>
       </c>
       <c r="D2">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E2">
-        <v>2500</v>
+        <v>1</v>
       </c>
       <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="H2" t="str">
+        <v>تعریف نشده</v>
+      </c>
+      <c r="I2" t="str">
+        <v/>
+      </c>
+      <c r="J2" t="str">
+        <v/>
+      </c>
+      <c r="K2" t="str">
+        <v>Irancell</v>
+      </c>
+      <c r="M2" t="b">
+        <v>0</v>
+      </c>
+      <c r="N2" t="b">
+        <v>1</v>
+      </c>
+      <c r="O2" t="str">
+        <v>new</v>
+      </c>
+      <c r="P2" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q2" t="str">
+        <v>659d7d342136954fd03e46d2</v>
+      </c>
+      <c r="R2" s="1">
+        <v>45300.85954648148</v>
+      </c>
+      <c r="S2" s="1">
+        <v>45300.85954648148</v>
+      </c>
+      <c r="T2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3">
+        <v>9125004913</v>
+      </c>
+      <c r="B3" t="str">
+        <v>0912  500 4900</v>
+      </c>
+      <c r="C3">
+        <v>17000</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="H3" t="str">
+        <v>تعریف نشده</v>
+      </c>
+      <c r="I3" t="str">
+        <v/>
+      </c>
+      <c r="J3" t="str">
+        <v/>
+      </c>
+      <c r="K3" t="str">
+        <v>Irancell</v>
+      </c>
+      <c r="M3" t="b">
+        <v>0</v>
+      </c>
+      <c r="N3" t="b">
+        <v>0</v>
+      </c>
+      <c r="O3" t="str">
+        <v>used</v>
+      </c>
+      <c r="P3" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q3" t="str">
+        <v>659d7d342136954fd03e46e0</v>
+      </c>
+      <c r="R3" s="1">
+        <v>45300.85954653935</v>
+      </c>
+      <c r="S3" s="1">
+        <v>45300.85954653935</v>
+      </c>
+      <c r="T3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4">
+        <v>9125004914</v>
+      </c>
+      <c r="B4" t="str">
+        <v>0912  500 4900</v>
+      </c>
+      <c r="C4">
+        <v>9500</v>
+      </c>
+      <c r="D4">
         <v>3</v>
       </c>
-      <c r="H2" t="str">
-        <v>فوری</v>
-      </c>
-      <c r="I2" t="str">
-        <v>لورم ایپسوم متن ساختگی با تولید سادگی نامفهوم از صنعت چاپ، و با استفاده از طراحان گرافیک است، چاپگرها و متون بلکه روزنامه و مجله در ستون و سطرآنچنان که لازم است، و برای شرایط فعلی تکنولوژی مورد نیاز، و کاربردهای متنوع با هدف بهبود ابزارهای کاربردی می باشد، کتابهای زیادی در شصت و سه درصد گذشته حال و آینده، شناخت فراوان جامعه و متخصصان را می طلبد، تا با نرم افزارها شناخت بیشتری را برای طراحان رایانه ای علی الخصوص طراحان خلاقی، و فرهنگ پیشرو در زبان فارسی ایجاد کرد، در این صورت می توان امید داشت که تمام و دشواری موجود در ارائه راهکارها، و شرایط سخت تایپ به پایان رسد و زمان مورد نیاز شامل حروفچینی دستاوردهای اصلی، و جوابگوی سوالات پیوسته اهل دنیای موجود طراحی اساسا مورد استفاده قرار گیرد.</v>
-      </c>
-      <c r="J2" t="str">
-        <v>آینه ای</v>
-      </c>
-      <c r="K2" t="str">
+      <c r="E4">
+        <v>2</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="H4" t="str">
+        <v>تعریف نشده</v>
+      </c>
+      <c r="I4" t="str">
+        <v/>
+      </c>
+      <c r="J4" t="str">
+        <v/>
+      </c>
+      <c r="K4" t="str">
         <v>Hamrah-e Aval</v>
       </c>
-      <c r="L2" s="1">
-        <v>45300.14634259259</v>
-      </c>
-      <c r="M2" t="b">
-        <v>1</v>
-      </c>
-      <c r="N2" t="b">
-        <v>1</v>
-      </c>
-      <c r="O2" t="str">
+      <c r="M4" t="b">
+        <v>0</v>
+      </c>
+      <c r="N4" t="b">
+        <v>0</v>
+      </c>
+      <c r="O4" t="str">
         <v>used</v>
       </c>
-      <c r="P2" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q2" t="str">
-        <v>6598e4d0c70f02721933a2be</v>
-      </c>
-      <c r="R2" s="1">
-        <v>45297.37393828703</v>
-      </c>
-      <c r="S2" s="1">
-        <v>45297.37916582176</v>
-      </c>
-      <c r="T2">
+      <c r="P4" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q4" t="str">
+        <v>659d7d342136954fd03e46e1</v>
+      </c>
+      <c r="R4" s="1">
+        <v>45300.85954655093</v>
+      </c>
+      <c r="S4" s="1">
+        <v>45300.85954655093</v>
+      </c>
+      <c r="T4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5">
+        <v>9125004915</v>
+      </c>
+      <c r="B5" t="str">
+        <v>0912  500 4900</v>
+      </c>
+      <c r="C5">
+        <v>6000</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>3</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="H5" t="str">
+        <v>تعریف نشده</v>
+      </c>
+      <c r="I5" t="str">
+        <v/>
+      </c>
+      <c r="J5" t="str">
+        <v/>
+      </c>
+      <c r="K5" t="str">
+        <v>Rightel</v>
+      </c>
+      <c r="M5" t="b">
+        <v>0</v>
+      </c>
+      <c r="N5" t="b">
+        <v>1</v>
+      </c>
+      <c r="O5" t="str">
+        <v>semi used</v>
+      </c>
+      <c r="P5" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q5" t="str">
+        <v>659d7d342136954fd03e46e2</v>
+      </c>
+      <c r="R5" s="1">
+        <v>45300.85954655093</v>
+      </c>
+      <c r="S5" s="1">
+        <v>45300.85954655093</v>
+      </c>
+      <c r="T5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6">
+        <v>9125004916</v>
+      </c>
+      <c r="B6" t="str">
+        <v>0912  500 4900</v>
+      </c>
+      <c r="C6">
+        <v>14000</v>
+      </c>
+      <c r="D6">
+        <v>2</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="H6" t="str">
+        <v>تعریف نشده</v>
+      </c>
+      <c r="I6" t="str">
+        <v/>
+      </c>
+      <c r="J6" t="str">
+        <v/>
+      </c>
+      <c r="K6" t="str">
+        <v>Irancell</v>
+      </c>
+      <c r="M6" t="b">
+        <v>0</v>
+      </c>
+      <c r="N6" t="b">
+        <v>1</v>
+      </c>
+      <c r="O6" t="str">
+        <v>semi used</v>
+      </c>
+      <c r="P6" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q6" t="str">
+        <v>659d7d342136954fd03e46e3</v>
+      </c>
+      <c r="R6" s="1">
+        <v>45300.8595465625</v>
+      </c>
+      <c r="S6" s="1">
+        <v>45300.86365939815</v>
+      </c>
+      <c r="T6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7">
+        <v>9125004917</v>
+      </c>
+      <c r="B7" t="str">
+        <v>0912  500 4900</v>
+      </c>
+      <c r="C7">
+        <v>11000</v>
+      </c>
+      <c r="D7">
+        <v>3</v>
+      </c>
+      <c r="E7">
+        <v>2</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="H7" t="str">
+        <v>تعریف نشده</v>
+      </c>
+      <c r="I7" t="str">
+        <v/>
+      </c>
+      <c r="J7" t="str">
+        <v/>
+      </c>
+      <c r="K7" t="str">
+        <v>Hamrah-e Aval</v>
+      </c>
+      <c r="M7" t="b">
+        <v>0</v>
+      </c>
+      <c r="N7" t="b">
+        <v>1</v>
+      </c>
+      <c r="O7" t="str">
+        <v>semi used</v>
+      </c>
+      <c r="P7" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q7" t="str">
+        <v>659d7d342136954fd03e46e4</v>
+      </c>
+      <c r="R7" s="1">
+        <v>45300.8595465625</v>
+      </c>
+      <c r="S7" s="1">
+        <v>45300.86366365741</v>
+      </c>
+      <c r="T7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8">
+        <v>9125004918</v>
+      </c>
+      <c r="B8" t="str">
+        <v>0912  500 4900</v>
+      </c>
+      <c r="C8">
+        <v>12000</v>
+      </c>
+      <c r="D8">
+        <v>2</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="H8" t="str">
+        <v>تعریف نشده</v>
+      </c>
+      <c r="I8" t="str">
+        <v/>
+      </c>
+      <c r="J8" t="str">
+        <v/>
+      </c>
+      <c r="K8" t="str">
+        <v>Rightel</v>
+      </c>
+      <c r="M8" t="b">
+        <v>0</v>
+      </c>
+      <c r="N8" t="b">
+        <v>1</v>
+      </c>
+      <c r="O8" t="str">
+        <v>semi used</v>
+      </c>
+      <c r="P8" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q8" t="str">
+        <v>659d7d342136954fd03e46e5</v>
+      </c>
+      <c r="R8" s="1">
+        <v>45300.85954657407</v>
+      </c>
+      <c r="S8" s="1">
+        <v>45300.863654872686</v>
+      </c>
+      <c r="T8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9">
+        <v>9125004912</v>
+      </c>
+      <c r="B9" t="str">
+        <v>0912  500 4900</v>
+      </c>
+      <c r="C9">
+        <v>10000</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>3</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="H9" t="str">
+        <v>تعریف نشده</v>
+      </c>
+      <c r="I9" t="str">
+        <v/>
+      </c>
+      <c r="J9" t="str">
+        <v/>
+      </c>
+      <c r="K9" t="str">
+        <v>Rightel</v>
+      </c>
+      <c r="M9" t="b">
+        <v>0</v>
+      </c>
+      <c r="N9" t="b">
+        <v>0</v>
+      </c>
+      <c r="O9" t="str">
+        <v>used</v>
+      </c>
+      <c r="P9" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q9" t="str">
+        <v>659d7d342136954fd03e46df</v>
+      </c>
+      <c r="R9" s="1">
+        <v>45300.85954653935</v>
+      </c>
+      <c r="S9" s="1">
+        <v>45300.85954653935</v>
+      </c>
+      <c r="T9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10">
+        <v>9125004902</v>
+      </c>
+      <c r="B10" t="str">
+        <v>0912  500 4900</v>
+      </c>
+      <c r="C10">
+        <v>18000</v>
+      </c>
+      <c r="D10">
+        <v>3</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="H10" t="str">
+        <v>تعریف نشده</v>
+      </c>
+      <c r="I10" t="str">
+        <v/>
+      </c>
+      <c r="J10" t="str">
+        <v/>
+      </c>
+      <c r="K10" t="str">
+        <v>Rightel</v>
+      </c>
+      <c r="M10" t="b">
+        <v>0</v>
+      </c>
+      <c r="N10" t="b">
+        <v>0</v>
+      </c>
+      <c r="O10" t="str">
+        <v>used</v>
+      </c>
+      <c r="P10" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q10" t="str">
+        <v>659d7d342136954fd03e46d5</v>
+      </c>
+      <c r="R10" s="1">
+        <v>45300.85954648148</v>
+      </c>
+      <c r="S10" s="1">
+        <v>45300.85954648148</v>
+      </c>
+      <c r="T10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11">
+        <v>9125004901</v>
+      </c>
+      <c r="B11" t="str">
+        <v>0912  500 4900</v>
+      </c>
+      <c r="C11">
+        <v>5000</v>
+      </c>
+      <c r="D11">
+        <v>2</v>
+      </c>
+      <c r="E11">
+        <v>2</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="H11" t="str">
+        <v>تعریف نشده</v>
+      </c>
+      <c r="I11" t="str">
+        <v/>
+      </c>
+      <c r="J11" t="str">
+        <v/>
+      </c>
+      <c r="K11" t="str">
+        <v>Hamrah-e Aval</v>
+      </c>
+      <c r="M11" t="b">
+        <v>0</v>
+      </c>
+      <c r="N11" t="b">
+        <v>1</v>
+      </c>
+      <c r="O11" t="str">
+        <v>used</v>
+      </c>
+      <c r="P11" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q11" t="str">
+        <v>659d7d342136954fd03e46d4</v>
+      </c>
+      <c r="R11" s="1">
+        <v>45300.859546493055</v>
+      </c>
+      <c r="S11" s="1">
+        <v>45300.859546493055</v>
+      </c>
+      <c r="T11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12">
+        <v>9125004903</v>
+      </c>
+      <c r="B12" t="str">
+        <v>0912  500 4900</v>
+      </c>
+      <c r="C12">
+        <v>10000</v>
+      </c>
+      <c r="D12">
+        <v>2</v>
+      </c>
+      <c r="E12">
+        <v>2</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="H12" t="str">
+        <v>تعریف نشده</v>
+      </c>
+      <c r="I12" t="str">
+        <v/>
+      </c>
+      <c r="J12" t="str">
+        <v/>
+      </c>
+      <c r="K12" t="str">
+        <v>Irancell</v>
+      </c>
+      <c r="M12" t="b">
+        <v>0</v>
+      </c>
+      <c r="N12" t="b">
+        <v>0</v>
+      </c>
+      <c r="O12" t="str">
+        <v>used</v>
+      </c>
+      <c r="P12" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q12" t="str">
+        <v>659d7d342136954fd03e46d6</v>
+      </c>
+      <c r="R12" s="1">
+        <v>45300.859546493055</v>
+      </c>
+      <c r="S12" s="1">
+        <v>45300.859546493055</v>
+      </c>
+      <c r="T12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13">
+        <v>9125004904</v>
+      </c>
+      <c r="B13" t="str">
+        <v>0912  500 4900</v>
+      </c>
+      <c r="C13">
+        <v>9000</v>
+      </c>
+      <c r="D13">
+        <v>2</v>
+      </c>
+      <c r="E13">
+        <v>2</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="H13" t="str">
+        <v>تعریف نشده</v>
+      </c>
+      <c r="I13" t="str">
+        <v/>
+      </c>
+      <c r="J13" t="str">
+        <v/>
+      </c>
+      <c r="K13" t="str">
+        <v>Irancell</v>
+      </c>
+      <c r="M13" t="b">
+        <v>0</v>
+      </c>
+      <c r="N13" t="b">
+        <v>0</v>
+      </c>
+      <c r="O13" t="str">
+        <v>used</v>
+      </c>
+      <c r="P13" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q13" t="str">
+        <v>659d7d342136954fd03e46d7</v>
+      </c>
+      <c r="R13" s="1">
+        <v>45300.85954650463</v>
+      </c>
+      <c r="S13" s="1">
+        <v>45300.85954650463</v>
+      </c>
+      <c r="T13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14">
+        <v>9125004906</v>
+      </c>
+      <c r="B14" t="str">
+        <v>0912  500 4900</v>
+      </c>
+      <c r="C14">
+        <v>7000</v>
+      </c>
+      <c r="D14">
+        <v>2</v>
+      </c>
+      <c r="E14">
+        <v>2</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="H14" t="str">
+        <v>تعریف نشده</v>
+      </c>
+      <c r="I14" t="str">
+        <v/>
+      </c>
+      <c r="J14" t="str">
+        <v/>
+      </c>
+      <c r="K14" t="str">
+        <v>Rightel</v>
+      </c>
+      <c r="M14" t="b">
+        <v>0</v>
+      </c>
+      <c r="N14" t="b">
+        <v>1</v>
+      </c>
+      <c r="O14" t="str">
+        <v>semi used</v>
+      </c>
+      <c r="P14" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q14" t="str">
+        <v>659d7d342136954fd03e46d9</v>
+      </c>
+      <c r="R14" s="1">
+        <v>45300.85954650463</v>
+      </c>
+      <c r="S14" s="1">
+        <v>45300.85954650463</v>
+      </c>
+      <c r="T14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15">
+        <v>9125004905</v>
+      </c>
+      <c r="B15" t="str">
+        <v>0912  500 4900</v>
+      </c>
+      <c r="C15">
+        <v>15000</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
+      <c r="H15" t="str">
+        <v>تعریف نشده</v>
+      </c>
+      <c r="I15" t="str">
+        <v/>
+      </c>
+      <c r="J15" t="str">
+        <v/>
+      </c>
+      <c r="K15" t="str">
+        <v>Hamrah-e Aval</v>
+      </c>
+      <c r="M15" t="b">
+        <v>0</v>
+      </c>
+      <c r="N15" t="b">
+        <v>1</v>
+      </c>
+      <c r="O15" t="str">
+        <v>semi used</v>
+      </c>
+      <c r="P15" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q15" t="str">
+        <v>659d7d342136954fd03e46d8</v>
+      </c>
+      <c r="R15" s="1">
+        <v>45300.85954651621</v>
+      </c>
+      <c r="S15" s="1">
+        <v>45300.85954651621</v>
+      </c>
+      <c r="T15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16">
+        <v>9125004907</v>
+      </c>
+      <c r="B16" t="str">
+        <v>0912  500 4900</v>
+      </c>
+      <c r="C16">
+        <v>16000</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
+      <c r="H16" t="str">
+        <v>تعریف نشده</v>
+      </c>
+      <c r="I16" t="str">
+        <v/>
+      </c>
+      <c r="J16" t="str">
+        <v/>
+      </c>
+      <c r="K16" t="str">
+        <v>Hamrah-e Aval</v>
+      </c>
+      <c r="M16" t="b">
+        <v>0</v>
+      </c>
+      <c r="N16" t="b">
+        <v>1</v>
+      </c>
+      <c r="O16" t="str">
+        <v>semi used</v>
+      </c>
+      <c r="P16" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q16" t="str">
+        <v>659d7d342136954fd03e46da</v>
+      </c>
+      <c r="R16" s="1">
+        <v>45300.85954651621</v>
+      </c>
+      <c r="S16" s="1">
+        <v>45300.85954651621</v>
+      </c>
+      <c r="T16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17">
+        <v>9125004908</v>
+      </c>
+      <c r="B17" t="str">
+        <v>0912  500 4900</v>
+      </c>
+      <c r="C17">
+        <v>12000</v>
+      </c>
+      <c r="D17">
+        <v>3</v>
+      </c>
+      <c r="E17">
+        <v>2</v>
+      </c>
+      <c r="F17">
+        <v>1</v>
+      </c>
+      <c r="H17" t="str">
+        <v>تعریف نشده</v>
+      </c>
+      <c r="I17" t="str">
+        <v/>
+      </c>
+      <c r="J17" t="str">
+        <v/>
+      </c>
+      <c r="K17" t="str">
+        <v>Irancell</v>
+      </c>
+      <c r="M17" t="b">
+        <v>0</v>
+      </c>
+      <c r="N17" t="b">
+        <v>1</v>
+      </c>
+      <c r="O17" t="str">
+        <v>new</v>
+      </c>
+      <c r="P17" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q17" t="str">
+        <v>659d7d342136954fd03e46db</v>
+      </c>
+      <c r="R17" s="1">
+        <v>45300.859546527776</v>
+      </c>
+      <c r="S17" s="1">
+        <v>45300.859546527776</v>
+      </c>
+      <c r="T17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18">
+        <v>9125004909</v>
+      </c>
+      <c r="B18" t="str">
+        <v>0912  500 4900</v>
+      </c>
+      <c r="C18">
+        <v>8000</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18">
+        <v>3</v>
+      </c>
+      <c r="F18">
+        <v>1</v>
+      </c>
+      <c r="H18" t="str">
+        <v>تعریف نشده</v>
+      </c>
+      <c r="I18" t="str">
+        <v/>
+      </c>
+      <c r="J18" t="str">
+        <v/>
+      </c>
+      <c r="K18" t="str">
+        <v>Rightel</v>
+      </c>
+      <c r="M18" t="b">
+        <v>0</v>
+      </c>
+      <c r="N18" t="b">
+        <v>1</v>
+      </c>
+      <c r="O18" t="str">
+        <v>new</v>
+      </c>
+      <c r="P18" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q18" t="str">
+        <v>659d7d342136954fd03e46dc</v>
+      </c>
+      <c r="R18" s="1">
+        <v>45300.859546527776</v>
+      </c>
+      <c r="S18" s="1">
+        <v>45300.859546527776</v>
+      </c>
+      <c r="T18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19">
+        <v>9125004910</v>
+      </c>
+      <c r="B19" t="str">
+        <v>0912  500 4900</v>
+      </c>
+      <c r="C19">
+        <v>11000</v>
+      </c>
+      <c r="D19">
+        <v>2</v>
+      </c>
+      <c r="E19">
+        <v>2</v>
+      </c>
+      <c r="F19">
+        <v>1</v>
+      </c>
+      <c r="H19" t="str">
+        <v>تعریف نشده</v>
+      </c>
+      <c r="I19" t="str">
+        <v/>
+      </c>
+      <c r="J19" t="str">
+        <v/>
+      </c>
+      <c r="K19" t="str">
+        <v>Irancell</v>
+      </c>
+      <c r="M19" t="b">
+        <v>0</v>
+      </c>
+      <c r="N19" t="b">
+        <v>0</v>
+      </c>
+      <c r="O19" t="str">
+        <v>new</v>
+      </c>
+      <c r="P19" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q19" t="str">
+        <v>659d7d342136954fd03e46dd</v>
+      </c>
+      <c r="R19" s="1">
+        <v>45300.859546527776</v>
+      </c>
+      <c r="S19" s="1">
+        <v>45300.859546527776</v>
+      </c>
+      <c r="T19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20">
+        <v>9125004911</v>
+      </c>
+      <c r="B20" t="str">
+        <v>0912  500 4900</v>
+      </c>
+      <c r="C20">
+        <v>13000</v>
+      </c>
+      <c r="D20">
+        <v>3</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+      <c r="F20">
+        <v>1</v>
+      </c>
+      <c r="H20" t="str">
+        <v>تعریف نشده</v>
+      </c>
+      <c r="I20" t="str">
+        <v/>
+      </c>
+      <c r="J20" t="str">
+        <v/>
+      </c>
+      <c r="K20" t="str">
+        <v>Hamrah-e Aval</v>
+      </c>
+      <c r="M20" t="b">
+        <v>0</v>
+      </c>
+      <c r="N20" t="b">
+        <v>0</v>
+      </c>
+      <c r="O20" t="str">
+        <v>new</v>
+      </c>
+      <c r="P20" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q20" t="str">
+        <v>659d7d342136954fd03e46de</v>
+      </c>
+      <c r="R20" s="1">
+        <v>45300.85954653935</v>
+      </c>
+      <c r="S20" s="1">
+        <v>45300.85954653935</v>
+      </c>
+      <c r="T20">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:T2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:T20"/>
   </ignoredErrors>
   <legacyDrawing r:id="rId1"/>
 </worksheet>

</xml_diff>